<commit_message>
Update test model '1_coupled_model'.
</commit_message>
<xml_diff>
--- a/tests/models/integrated/1_coupled_model/model_settings.xlsx
+++ b/tests/models/integrated/1_coupled_model/model_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\models\integrated\1_coupled_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD990821-3E98-4C64-9972-A71C651C23E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28AFD02-90F5-444D-A928-4FCA652F2259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37640" yWindow="760" windowWidth="28800" windowHeight="15370" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="structure_sets" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>set_key</t>
   </si>
@@ -165,6 +165,18 @@
   </si>
   <si>
     <t>category: [energy_use_0, learning_rate, profit]</t>
+  </si>
+  <si>
+    <t>maximization of total profit</t>
+  </si>
+  <si>
+    <t>energy use less than endowment</t>
+  </si>
+  <si>
+    <t>positive products supply</t>
+  </si>
+  <si>
+    <t>energy use per unit of product</t>
   </si>
 </sst>
 </file>
@@ -261,12 +273,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9E7FEE58-959B-4A76-BD2C-C7A4A140E173}" name="Table4" displayName="Table4" ref="A1:C5" totalsRowShown="0">
-  <autoFilter ref="A1:C5" xr:uid="{9E7FEE58-959B-4A76-BD2C-C7A4A140E173}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9E7FEE58-959B-4A76-BD2C-C7A4A140E173}" name="Table4" displayName="Table4" ref="A1:D5" totalsRowShown="0">
+  <autoFilter ref="A1:D5" xr:uid="{9E7FEE58-959B-4A76-BD2C-C7A4A140E173}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{339B6BC6-DC77-44F3-BC7D-5887B7C1C68A}" name="problem_key" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{7D3A5DDD-E4D2-4BFD-8F61-20DAAF76C565}" name="objective"/>
     <tableColumn id="3" xr3:uid="{F83410DB-FD97-4F82-A158-44491E25E434}" name="expressions"/>
+    <tableColumn id="4" xr3:uid="{9BA42D33-7C36-4CDA-8AAE-32BCE0C105B1}" name="description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -797,10 +810,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB4DB9B-67B8-45E9-9CD6-D02B1BE46AE7}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -808,9 +821,10 @@
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.08984375" customWidth="1"/>
     <col min="3" max="3" width="23.90625" customWidth="1"/>
+    <col min="4" max="4" width="30.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -820,37 +834,52 @@
       <c r="C1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>